<commit_message>
Updated mode class and types
</commit_message>
<xml_diff>
--- a/model_class_and_types.xlsx
+++ b/model_class_and_types.xlsx
@@ -5,17 +5,18 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/icaoberg/Desktop/temp/cellorganizer-docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/icaoberg/Desktop/cellorganizer-docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="19540" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="v2.7" sheetId="3" r:id="rId1"/>
-    <sheet name="v2.6" sheetId="4" r:id="rId2"/>
-    <sheet name="v2.5" sheetId="1" r:id="rId3"/>
-    <sheet name="2D-3D" sheetId="2" r:id="rId4"/>
+    <sheet name="v2.7.1" sheetId="5" r:id="rId1"/>
+    <sheet name="v2.7" sheetId="3" r:id="rId2"/>
+    <sheet name="v2.6" sheetId="4" r:id="rId3"/>
+    <sheet name="v2.5" sheetId="1" r:id="rId4"/>
+    <sheet name="2D-3D" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="41">
   <si>
     <t>2D/3D</t>
   </si>
@@ -153,6 +154,9 @@
   </si>
   <si>
     <t>half-ellipsoid</t>
+  </si>
+  <si>
+    <t>pca</t>
   </si>
 </sst>
 </file>
@@ -217,6 +221,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table1346" displayName="Table1346" ref="A1:E11" totalsRowShown="0">
+  <autoFilter ref="A1:E11"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="2D/3D"/>
+    <tableColumn id="2" name="Model Class"/>
+    <tableColumn id="3" name="Model Type"/>
+    <tableColumn id="4" name="Depends on"/>
+    <tableColumn id="5" name="Produces"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table134" displayName="Table134" ref="A1:E10" totalsRowShown="0">
   <autoFilter ref="A1:E10"/>
   <tableColumns count="5">
@@ -230,7 +248,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table135" displayName="Table135" ref="A1:E10" totalsRowShown="0">
   <autoFilter ref="A1:E10"/>
   <tableColumns count="5">
@@ -244,7 +262,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:E10" totalsRowShown="0">
   <autoFilter ref="A1:E10"/>
   <tableColumns count="5">
@@ -258,7 +276,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G11" totalsRowShown="0">
   <autoFilter ref="A1:G11"/>
   <tableColumns count="7">
@@ -599,10 +617,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -660,33 +678,30 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -694,13 +709,16 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -708,35 +726,35 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
@@ -753,16 +771,13 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -770,13 +785,16 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>19</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
       </c>
       <c r="E11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -784,10 +802,13 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>22</v>
+      </c>
+      <c r="E12" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -795,9 +816,20 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
         <v>38</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>39</v>
       </c>
     </row>
@@ -814,10 +846,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -992,6 +1024,28 @@
       </c>
       <c r="E11" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1200,6 +1254,199 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Updated model class and types
</commit_message>
<xml_diff>
--- a/model_class_and_types.xlsx
+++ b/model_class_and_types.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14120" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="v2.8.0" sheetId="7" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="44">
   <si>
     <t>2D/3D</t>
   </si>
@@ -154,6 +154,15 @@
   </si>
   <si>
     <t>pca</t>
+  </si>
+  <si>
+    <t>SPHARM</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>cell membrane, nuclear membrane</t>
   </si>
 </sst>
 </file>
@@ -645,10 +654,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -859,6 +868,23 @@
       </c>
       <c r="C14" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>